<commit_message>
Filter2 prototype - change some component values
</commit_message>
<xml_diff>
--- a/modules/Filter2/prototype/prototype-BOM.xlsx
+++ b/modules/Filter2/prototype/prototype-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Filter2\prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65652F18-3D48-43A5-82B4-042A63B069E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B3B8D9-E148-4608-906D-18B14AEDB6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1080" windowWidth="18540" windowHeight="12495"/>
+    <workbookView xWindow="4050" yWindow="2145" windowWidth="18540" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prototype-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="101">
   <si>
     <t>Ref</t>
   </si>
@@ -88,9 +101,6 @@
     <t>C2 C3</t>
   </si>
   <si>
-    <t>6N8</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -166,9 +176,6 @@
     <t>100K</t>
   </si>
   <si>
-    <t>R3 R9 R12 R13</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -184,21 +191,9 @@
     <t>1K</t>
   </si>
   <si>
-    <t>R7 R8</t>
-  </si>
-  <si>
     <t>15K</t>
   </si>
   <si>
-    <t>R10 R11</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
     <t>51R</t>
   </si>
   <si>
@@ -325,19 +320,28 @@
     <t>Need</t>
   </si>
   <si>
-    <t>sub 1U</t>
-  </si>
-  <si>
     <t>sub 18PF</t>
   </si>
   <si>
     <t>sub 100K</t>
+  </si>
+  <si>
+    <t>1N2</t>
+  </si>
+  <si>
+    <t>R3 R9</t>
+  </si>
+  <si>
+    <t>R7 R8 R12 R13</t>
+  </si>
+  <si>
+    <t>R10 R11 R16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1183,15 +1187,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="4.140625" customWidth="1"/>
   </cols>
@@ -1204,13 +1209,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1293,14 +1298,11 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E18" si="0">MAX(0,B3-C3-D3)</f>
+        <f t="shared" ref="E3:E17" si="0">MAX(0,B3-C3-D3)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
         <v>20</v>
@@ -1308,7 +1310,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1321,21 +1323,21 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
         <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1348,36 +1350,36 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
         <v>28</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>34</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1390,36 +1392,36 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>39</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>41</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
         <v>43</v>
       </c>
-      <c r="M6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>44</v>
-      </c>
-      <c r="O6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1432,39 +1434,39 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>41</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>42</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
         <v>43</v>
       </c>
-      <c r="M7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>44</v>
-      </c>
-      <c r="O7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1474,36 +1476,36 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
         <v>39</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>40</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>41</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>42</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" t="s">
         <v>43</v>
       </c>
-      <c r="M8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>44</v>
-      </c>
-      <c r="O8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1516,36 +1518,36 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
         <v>39</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>40</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>41</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" t="s">
         <v>43</v>
       </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>44</v>
-      </c>
-      <c r="O9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1558,276 +1560,273 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="s">
         <v>39</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>40</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>41</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>42</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" t="s">
         <v>43</v>
       </c>
-      <c r="M10" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>44</v>
-      </c>
-      <c r="O10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s">
         <v>39</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>40</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>41</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>42</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" t="s">
         <v>43</v>
       </c>
-      <c r="M11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>44</v>
-      </c>
-      <c r="O11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" t="s">
-        <v>44</v>
-      </c>
       <c r="O12" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>1</v>
+      <c r="D13">
+        <v>3</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" t="s">
         <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" t="s">
         <v>62</v>
-      </c>
-      <c r="M13" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" t="s">
-        <v>63</v>
-      </c>
-      <c r="O13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>3</v>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" t="s">
         <v>66</v>
       </c>
-      <c r="G14" t="s">
+      <c r="L14" t="s">
         <v>67</v>
       </c>
-      <c r="I14" t="s">
+      <c r="M14" t="s">
         <v>68</v>
+      </c>
+      <c r="N14" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" t="s">
+        <v>70</v>
+      </c>
+      <c r="P14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>71</v>
+      </c>
+      <c r="R14" t="s">
+        <v>72</v>
+      </c>
+      <c r="S14" t="s">
+        <v>73</v>
+      </c>
+      <c r="T14" t="s">
+        <v>74</v>
+      </c>
+      <c r="U14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>1</v>
+      <c r="D15">
+        <v>3</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" t="s">
-        <v>71</v>
-      </c>
-      <c r="K15" t="s">
-        <v>72</v>
-      </c>
-      <c r="L15" t="s">
-        <v>73</v>
-      </c>
-      <c r="M15" t="s">
-        <v>74</v>
-      </c>
-      <c r="N15" t="s">
-        <v>75</v>
-      </c>
-      <c r="O15" t="s">
-        <v>76</v>
-      </c>
-      <c r="P15" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>77</v>
-      </c>
-      <c r="R15" t="s">
-        <v>78</v>
-      </c>
-      <c r="S15" t="s">
-        <v>79</v>
-      </c>
-      <c r="T15" t="s">
-        <v>80</v>
-      </c>
-      <c r="U15" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="D16">
-        <v>3</v>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c r="J16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" t="s">
+        <v>83</v>
+      </c>
+      <c r="O16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1840,71 +1839,32 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
         <v>91</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" t="s">
-        <v>93</v>
-      </c>
-      <c r="J18" t="s">
-        <v>94</v>
-      </c>
-      <c r="K18" t="s">
-        <v>87</v>
-      </c>
-      <c r="L18" t="s">
-        <v>95</v>
-      </c>
-      <c r="M18" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" t="s">
-        <v>96</v>
-      </c>
-      <c r="O18" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E18">
+  <conditionalFormatting sqref="E2:E17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>